<commit_message>
20200901 23:03 Modify Css
</commit_message>
<xml_diff>
--- a/backend_python/data/재무제표.xlsx
+++ b/backend_python/data/재무제표.xlsx
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -977,7 +977,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>22150</v>
+        <v>23450</v>
       </c>
       <c r="D2" s="1">
         <v>27931470</v>
@@ -1051,7 +1051,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="1">
-        <v>676</v>
+        <v>705</v>
       </c>
       <c r="D3" s="1">
         <v>91661018</v>
@@ -1125,7 +1125,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1">
-        <v>10850</v>
+        <v>10550</v>
       </c>
       <c r="D4" s="1">
         <v>27415270</v>
@@ -1199,7 +1199,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="1">
-        <v>38700</v>
+        <v>36900</v>
       </c>
       <c r="D5" s="1">
         <v>70133611</v>
@@ -1273,7 +1273,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>65800</v>
+        <v>67000</v>
       </c>
       <c r="D6" s="1">
         <v>66856810</v>
@@ -1347,7 +1347,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="1">
-        <v>148000</v>
+        <v>151500</v>
       </c>
       <c r="D7" s="1">
         <v>22812344</v>
@@ -1421,7 +1421,7 @@
         <v>33</v>
       </c>
       <c r="C8" s="1">
-        <v>42050</v>
+        <v>46450</v>
       </c>
       <c r="D8" s="1">
         <v>16523835</v>
@@ -1569,7 +1569,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="1">
-        <v>78800</v>
+        <v>86900</v>
       </c>
       <c r="D10" s="1">
         <v>34800000</v>
@@ -1643,7 +1643,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="1">
-        <v>17950</v>
+        <v>17000</v>
       </c>
       <c r="D11" s="1">
         <v>6902772</v>
@@ -1717,7 +1717,7 @@
         <v>54</v>
       </c>
       <c r="C12" s="1">
-        <v>41300</v>
+        <v>42450</v>
       </c>
       <c r="D12" s="1">
         <v>405363347</v>
@@ -1791,7 +1791,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="1">
-        <v>9100</v>
+        <v>9160</v>
       </c>
       <c r="D13" s="1">
         <v>13291151</v>
@@ -1865,7 +1865,7 @@
         <v>55</v>
       </c>
       <c r="C14" s="1">
-        <v>4845</v>
+        <v>5180</v>
       </c>
       <c r="D14" s="1">
         <v>26438751</v>
@@ -1939,7 +1939,7 @@
         <v>37</v>
       </c>
       <c r="C15" s="1">
-        <v>3050</v>
+        <v>3120</v>
       </c>
       <c r="D15" s="1">
         <v>62000000</v>
@@ -2013,7 +2013,7 @@
         <v>38</v>
       </c>
       <c r="C16" s="1">
-        <v>7870</v>
+        <v>7750</v>
       </c>
       <c r="D16" s="1">
         <v>6227130</v>
@@ -2087,7 +2087,7 @@
         <v>39</v>
       </c>
       <c r="C17" s="1">
-        <v>72400</v>
+        <v>72100</v>
       </c>
       <c r="D17" s="1">
         <v>4000000</v>
@@ -2235,7 +2235,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="1">
-        <v>19950</v>
+        <v>20800</v>
       </c>
       <c r="D19" s="1">
         <v>6500000</v>
@@ -2309,7 +2309,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="1">
-        <v>50900</v>
+        <v>55800</v>
       </c>
       <c r="D20" s="1">
         <v>1154482</v>
@@ -2383,7 +2383,7 @@
         <v>42</v>
       </c>
       <c r="C21" s="1">
-        <v>97800</v>
+        <v>108500</v>
       </c>
       <c r="D21" s="1">
         <v>6138297</v>
@@ -2457,7 +2457,7 @@
         <v>43</v>
       </c>
       <c r="C22" s="1">
-        <v>76300</v>
+        <v>75100</v>
       </c>
       <c r="D22" s="1">
         <v>728002365</v>
@@ -2531,7 +2531,7 @@
         <v>44</v>
       </c>
       <c r="C23" s="1">
-        <v>482500</v>
+        <v>489500</v>
       </c>
       <c r="D23" s="1">
         <v>1842040</v>
@@ -2605,7 +2605,7 @@
         <v>45</v>
       </c>
       <c r="C24" s="1">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="D24" s="1">
         <v>78803016</v>
@@ -2679,7 +2679,7 @@
         <v>46</v>
       </c>
       <c r="C25" s="1">
-        <v>14100</v>
+        <v>14700</v>
       </c>
       <c r="D25" s="1">
         <v>2800000</v>
@@ -2753,7 +2753,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="1">
-        <v>30450</v>
+        <v>30500</v>
       </c>
       <c r="D26" s="1">
         <v>2200000</v>
@@ -2827,7 +2827,7 @@
         <v>48</v>
       </c>
       <c r="C27" s="1">
-        <v>14650</v>
+        <v>15050</v>
       </c>
       <c r="D27" s="1">
         <v>6500000</v>
@@ -2901,7 +2901,7 @@
         <v>49</v>
       </c>
       <c r="C28" s="1">
-        <v>25400</v>
+        <v>27500</v>
       </c>
       <c r="D28" s="1">
         <v>74958735</v>
@@ -2975,7 +2975,7 @@
         <v>50</v>
       </c>
       <c r="C29" s="1">
-        <v>26250</v>
+        <v>28850</v>
       </c>
       <c r="D29" s="1">
         <v>1680000</v>
@@ -3049,7 +3049,7 @@
         <v>51</v>
       </c>
       <c r="C30" s="1">
-        <v>36600</v>
+        <v>35550</v>
       </c>
       <c r="D30" s="1">
         <v>44398588</v>
@@ -3123,7 +3123,7 @@
         <v>52</v>
       </c>
       <c r="C31" s="1">
-        <v>1405</v>
+        <v>1520</v>
       </c>
       <c r="D31" s="1">
         <v>35166280</v>
@@ -3197,7 +3197,7 @@
         <v>53</v>
       </c>
       <c r="C32" s="1">
-        <v>38200</v>
+        <v>38150</v>
       </c>
       <c r="D32" s="1">
         <v>20920054</v>
@@ -3271,7 +3271,7 @@
         <v>56</v>
       </c>
       <c r="C33" s="1">
-        <v>165500</v>
+        <v>171500</v>
       </c>
       <c r="D33" s="1">
         <v>1690000</v>
@@ -3345,7 +3345,7 @@
         <v>57</v>
       </c>
       <c r="C34" s="1">
-        <v>3155</v>
+        <v>3230</v>
       </c>
       <c r="D34" s="1">
         <v>11981820</v>
@@ -3419,7 +3419,7 @@
         <v>58</v>
       </c>
       <c r="C35" s="1">
-        <v>1630</v>
+        <v>1625</v>
       </c>
       <c r="D35" s="1">
         <v>82533764</v>
@@ -3493,7 +3493,7 @@
         <v>59</v>
       </c>
       <c r="C36" s="1">
-        <v>10150</v>
+        <v>10000</v>
       </c>
       <c r="D36" s="1">
         <v>9828611</v>
@@ -3567,7 +3567,7 @@
         <v>60</v>
       </c>
       <c r="C37" s="1">
-        <v>3510</v>
+        <v>3405</v>
       </c>
       <c r="D37" s="1">
         <v>44918407</v>
@@ -3641,7 +3641,7 @@
         <v>8</v>
       </c>
       <c r="C38" s="1">
-        <v>3695</v>
+        <v>3955</v>
       </c>
       <c r="D38" s="1">
         <v>61549713</v>
@@ -3715,7 +3715,7 @@
         <v>61</v>
       </c>
       <c r="C39" s="1">
-        <v>1780</v>
+        <v>1880</v>
       </c>
       <c r="D39" s="1">
         <v>44964143</v>
@@ -3789,7 +3789,7 @@
         <v>62</v>
       </c>
       <c r="C40" s="1">
-        <v>3315</v>
+        <v>3420</v>
       </c>
       <c r="D40" s="1">
         <v>7600000</v>
@@ -3863,7 +3863,7 @@
         <v>63</v>
       </c>
       <c r="C41" s="1">
-        <v>234500</v>
+        <v>244000</v>
       </c>
       <c r="D41" s="1">
         <v>624615</v>
@@ -3937,7 +3937,7 @@
         <v>64</v>
       </c>
       <c r="C42" s="1">
-        <v>907</v>
+        <v>952</v>
       </c>
       <c r="D42" s="1">
         <v>137546368</v>
@@ -4011,7 +4011,7 @@
         <v>65</v>
       </c>
       <c r="C43" s="1">
-        <v>92000</v>
+        <v>87700</v>
       </c>
       <c r="D43" s="1">
         <v>2465609</v>
@@ -4085,7 +4085,7 @@
         <v>66</v>
       </c>
       <c r="C44" s="1">
-        <v>6260</v>
+        <v>6360</v>
       </c>
       <c r="D44" s="1">
         <v>10000000</v>
@@ -4159,7 +4159,7 @@
         <v>67</v>
       </c>
       <c r="C45" s="1">
-        <v>4010</v>
+        <v>4300</v>
       </c>
       <c r="D45" s="1">
         <v>44048135</v>
@@ -4233,7 +4233,7 @@
         <v>68</v>
       </c>
       <c r="C46" s="1">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="D46" s="1">
         <v>66042072</v>
@@ -4381,7 +4381,7 @@
         <v>69</v>
       </c>
       <c r="C48" s="1">
-        <v>45150</v>
+        <v>46150</v>
       </c>
       <c r="D48" s="1">
         <v>9386237</v>
@@ -4455,7 +4455,7 @@
         <v>70</v>
       </c>
       <c r="C49" s="1">
-        <v>18600</v>
+        <v>18700</v>
       </c>
       <c r="D49" s="1">
         <v>8969658</v>
@@ -4529,7 +4529,7 @@
         <v>71</v>
       </c>
       <c r="C50" s="1">
-        <v>13500</v>
+        <v>13100</v>
       </c>
       <c r="D50" s="1">
         <v>62645422</v>
@@ -4603,7 +4603,7 @@
         <v>123</v>
       </c>
       <c r="C51" s="1">
-        <v>54900</v>
+        <v>54100</v>
       </c>
       <c r="D51" s="4">
         <v>10395000</v>

</xml_diff>